<commit_message>
Still working on use case 3
Scheduler still does not reads the excel files but Use Case 2 is working better than i expected
</commit_message>
<xml_diff>
--- a/myQfcProject/mycommon/src/main/resources/success.xlsx_error.xlsx
+++ b/myQfcProject/mycommon/src/main/resources/success.xlsx_error.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Error Data</t>
   </si>
@@ -29,16 +29,25 @@
     <t>File Name</t>
   </si>
   <si>
-    <t>1.0</t>
+    <t>sidd</t>
+  </si>
+  <si>
+    <t>Invalid numeric cell type</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>C:\Users\Siddharth Shinde\Desktop\Springmaven\myQfcProject\myQfcProject\mycommon\src\main\resources\success.xlsx</t>
+  </si>
+  <si>
+    <t>12.0</t>
   </si>
   <si>
     <t>Invalid string cell type</t>
   </si>
   <si>
     <t>UserName</t>
-  </si>
-  <si>
-    <t>C:\Users\Siddharth Shinde\Desktop\Springmaven\myQfcProject\myQfcProject\mycommon\src\main\resources\success.xlsx</t>
   </si>
 </sst>
 </file>
@@ -83,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -114,7 +123,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -123,6 +132,57 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>